<commit_message>
Improve stats reliability and UX: fix JSX and closing blocks; enforce mandatory columns (checkbox, actions, lrNo, lrDate, vehicleNo, status) and hide non-hideable from modal; align table cells with visible columns; remove Charts card, keep Filters visible; re-enable top stats cards; normalize status from API; aggressive refetch; mark API routes dynamic with no-store caching; fix build bailout for check-duplicate
</commit_message>
<xml_diff>
--- a/Additional Bill Format.xlsx
+++ b/Additional Bill Format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lr_billing_app_test\lr_billing_web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LRBillingOnline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6861FB70-E711-43F5-9986-0BD06C264465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263C6A0A-349C-4D5D-8F7B-FCA1E27F149D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="0" windowWidth="28530" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -144,7 +144,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:I8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,54 +487,19 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
@@ -546,27 +510,12 @@
     <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="3:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="3:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="3:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>